<commit_message>
Added flash messages and application skeleton in process
</commit_message>
<xml_diff>
--- a/docs/references.xlsx
+++ b/docs/references.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Dockerfile Commands</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>api</t>
+  </si>
+  <si>
+    <t>ejs</t>
+  </si>
+  <si>
+    <t>https://github.com/visionmedia/ejs#includes</t>
   </si>
 </sst>
 </file>
@@ -410,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D17"/>
+  <dimension ref="A3:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,12 +475,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -484,6 +500,7 @@
     <hyperlink ref="D11" r:id="rId3"/>
     <hyperlink ref="D16" r:id="rId4"/>
     <hyperlink ref="D17" r:id="rId5"/>
+    <hyperlink ref="D20" r:id="rId6" location="includes" display="https://github.com/visionmedia/ejs - includes"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>